<commit_message>
Working verified version 1.0
</commit_message>
<xml_diff>
--- a/misc/Payline Stats.xlsx
+++ b/misc/Payline Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Paylines</t>
   </si>
@@ -37,6 +37,45 @@
   </si>
   <si>
     <t>Note: Times are not for individual runs</t>
+  </si>
+  <si>
+    <t>jan</t>
+  </si>
+  <si>
+    <t>feb</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>apr</t>
+  </si>
+  <si>
+    <t>may</t>
+  </si>
+  <si>
+    <t>jun</t>
+  </si>
+  <si>
+    <t>jul</t>
+  </si>
+  <si>
+    <t>aug</t>
+  </si>
+  <si>
+    <t>sep</t>
+  </si>
+  <si>
+    <t>oct</t>
+  </si>
+  <si>
+    <t>nov</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -115,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -132,6 +171,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B2:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -453,7 +495,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -479,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>1</v>
       </c>
@@ -505,7 +547,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>2</v>
       </c>
@@ -531,7 +573,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -557,7 +599,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -583,7 +625,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>10</v>
       </c>
@@ -609,7 +651,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>15</v>
       </c>
@@ -635,7 +677,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
@@ -648,7 +690,90 @@
       <c r="I11" s="2"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="8">
+        <v>31</v>
+      </c>
+      <c r="D15" s="8">
+        <v>28</v>
+      </c>
+      <c r="E15" s="8">
+        <v>31</v>
+      </c>
+      <c r="F15" s="8">
+        <v>30</v>
+      </c>
+      <c r="G15" s="8">
+        <v>31</v>
+      </c>
+      <c r="H15" s="8">
+        <v>30</v>
+      </c>
+      <c r="I15" s="8">
+        <v>31</v>
+      </c>
+      <c r="J15" s="8">
+        <v>31</v>
+      </c>
+      <c r="K15" s="8">
+        <v>30</v>
+      </c>
+      <c r="L15" s="8">
+        <v>31</v>
+      </c>
+      <c r="M15" s="8">
+        <v>30</v>
+      </c>
+      <c r="N15" s="8">
+        <v>31</v>
+      </c>
+      <c r="O15">
+        <f>SUM(C15:N15)</f>
+        <v>365</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C2:E2"/>

</xml_diff>